<commit_message>
maj plan de tests
</commit_message>
<xml_diff>
--- a/Plan de tests.xlsx
+++ b/Plan de tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivierbasquin/Desktop/Olivierbasquin_5_26042021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E744DBBE-D533-C84E-A402-0AFCD2E9FA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D0D88-77F5-1F4F-A4B5-C209D56F8D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47980" yWindow="-14980" windowWidth="33060" windowHeight="24380" xr2:uid="{F08B11FB-A9AE-B04E-B17F-D9F01A7776E8}"/>
+    <workbookView xWindow="-90960" yWindow="-17840" windowWidth="35540" windowHeight="27720" xr2:uid="{F08B11FB-A9AE-B04E-B17F-D9F01A7776E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -401,6 +401,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1460500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{534A6D84-6A2B-0745-9EE2-D651EFD3E021}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11950700" y="6908800"/>
+          <a:ext cx="12700" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4315,5 +4364,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>